<commit_message>
Kiem thu dong dieu khien
</commit_message>
<xml_diff>
--- a/CinemaData.xlsx
+++ b/CinemaData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HI\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu20.04LTS\home\nguyenquynh1506\Testing\MochaTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11712" windowHeight="6564" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11712" windowHeight="6564" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="PH tương đương" sheetId="2" r:id="rId1"/>
-    <sheet name="Bảng Quyết định" sheetId="1" r:id="rId2"/>
+    <sheet name="Kiểm thử hộp đen_PH tương đương" sheetId="2" r:id="rId1"/>
+    <sheet name="Kiểm thử hộp đen_Bảng QĐ" sheetId="1" r:id="rId2"/>
+    <sheet name="Kiểm thử dòng điều khiển_Hàm 1" sheetId="3" r:id="rId3"/>
+    <sheet name="Kiểm thử dòng điều khiển_Hàm 2" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +87,15 @@
   </si>
   <si>
     <t>Next week</t>
+  </si>
+  <si>
+    <t>weekday</t>
+  </si>
+  <si>
+    <t>weekend</t>
+  </si>
+  <si>
+    <t>Input</t>
   </si>
 </sst>
 </file>
@@ -150,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -162,6 +173,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,7 +459,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -772,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -970,4 +984,153 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="19.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>25.5</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>16</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>45</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>70</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Kiem thu dong du lieu
</commit_message>
<xml_diff>
--- a/CinemaData.xlsx
+++ b/CinemaData.xlsx
@@ -9,13 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11712" windowHeight="6564" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11712" windowHeight="6564" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Kiểm thử hộp đen_PH tương đương" sheetId="2" r:id="rId1"/>
     <sheet name="Kiểm thử hộp đen_Bảng QĐ" sheetId="1" r:id="rId2"/>
     <sheet name="Kiểm thử dòng điều khiển_Hàm 1" sheetId="3" r:id="rId3"/>
     <sheet name="Kiểm thử dòng điều khiển_Hàm 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Kiểm thử dòng dữ liệu_Hàm 1" sheetId="7" r:id="rId5"/>
+    <sheet name="Kiểm thử dòng dữ liệu_Hàm 2" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="23">
   <si>
     <t>ID</t>
   </si>
@@ -458,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -1055,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1133,4 +1135,143 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="2">
+        <v>40</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2">
+        <v>20</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>